<commit_message>
added exception when double user
</commit_message>
<xml_diff>
--- a/ue01_useranlegen/Klassenraeume_2023.xlsx
+++ b/ue01_useranlegen/Klassenraeume_2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harald\SEW\SEW5-Skriptum\01_User_anlegen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/School/SEW/python/ue01_useranlegen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5378D8D-F5D5-4346-B13C-F5E551D41E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1069E4B8-A0BB-6649-BF62-746B5C638882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="25380" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aushang" sheetId="1" r:id="rId1"/>
@@ -609,7 +609,7 @@
     <cellStyle name=".3" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name=".error" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Ergebnis 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -738,7 +738,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1039,17 +1039,17 @@
   </sheetPr>
   <dimension ref="A1:AME42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C42" sqref="A42:C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1019" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1019" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1078,7 @@
       <c r="AMD1"/>
       <c r="AME1"/>
     </row>
-    <row r="2" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1103,7 +1103,7 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>33</v>
       </c>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:1019" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1019" ht="19" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
         <v>48</v>
       </c>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
         <v>51</v>
       </c>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A19" s="8" t="s">
         <v>54</v>
       </c>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
         <v>57</v>
       </c>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A21" s="8" t="s">
         <v>60</v>
       </c>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A22" s="8" t="s">
         <v>63</v>
       </c>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
         <v>66</v>
       </c>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A24" s="8" t="s">
         <v>69</v>
       </c>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A25" s="8" t="s">
         <v>72</v>
       </c>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A26" s="11" t="s">
         <v>75</v>
       </c>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="D26" s="13"/>
     </row>
-    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A27" s="11" t="s">
         <v>78</v>
       </c>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="D27" s="13"/>
     </row>
-    <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A28" s="11" t="s">
         <v>81</v>
       </c>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="D28" s="13"/>
     </row>
-    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A29" s="11" t="s">
         <v>84</v>
       </c>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="D29" s="13"/>
     </row>
-    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A30" s="11" t="s">
         <v>87</v>
       </c>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="D30" s="13"/>
     </row>
-    <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A31" s="11" t="s">
         <v>90</v>
       </c>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="D31" s="13"/>
     </row>
-    <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A32" s="11" t="s">
         <v>93</v>
       </c>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="D32" s="13"/>
     </row>
-    <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A33" s="11" t="s">
         <v>96</v>
       </c>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D33" s="13"/>
     </row>
-    <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A34" s="11" t="s">
         <v>99</v>
       </c>
@@ -1475,7 +1475,7 @@
       </c>
       <c r="D34" s="13"/>
     </row>
-    <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A35" s="11" t="s">
         <v>101</v>
       </c>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="D35" s="13"/>
     </row>
-    <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A36" s="11" t="s">
         <v>104</v>
       </c>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="D36" s="13"/>
     </row>
-    <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A37" s="11" t="s">
         <v>107</v>
       </c>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="D37" s="13"/>
     </row>
-    <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A38" s="11" t="s">
         <v>109</v>
       </c>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="D38" s="13"/>
     </row>
-    <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A39" s="11" t="s">
         <v>112</v>
       </c>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A40" s="11" t="s">
         <v>115</v>
       </c>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="D40" s="13"/>
     </row>
-    <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="19" x14ac:dyDescent="0.15">
       <c r="A41" s="14" t="s">
         <v>118</v>
       </c>
@@ -1559,7 +1559,7 @@
       </c>
       <c r="D41" s="15"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>

</xml_diff>